<commit_message>
Third Party Reservation Test is added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -4,11 +4,13 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Walk-In" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Koda" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet5" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Sheet2" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CarMake" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Sheet4" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="ThirdParty" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="ThirdPartySearchConfirmationNum" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Koda" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="Sheet5" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Sheet2" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="CarMake" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="Sheet4" sheetId="8" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -16,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="574" uniqueCount="199">
   <si>
     <t>Select Source</t>
   </si>
@@ -231,6 +233,21 @@
     <t>Il75503</t>
   </si>
   <si>
+    <t>confirmation Number</t>
+  </si>
+  <si>
+    <t>Prepaid Or Partial</t>
+  </si>
+  <si>
+    <t>CheapAirportParking</t>
+  </si>
+  <si>
+    <t>CHAP45615</t>
+  </si>
+  <si>
+    <t>Prepaid/Partial</t>
+  </si>
+  <si>
     <t>Reservation Prepaid</t>
   </si>
   <si>
@@ -238,9 +255,6 @@
   </si>
   <si>
     <t>Non Prepaid</t>
-  </si>
-  <si>
-    <t>Prepaid/Partial</t>
   </si>
   <si>
     <t>The Car_Make_DropDown_Option_List : Acura</t>
@@ -706,6 +720,14 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -1348,76 +1370,61 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="26.13"/>
+    <col customWidth="1" min="1" max="1" width="33.5"/>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
       <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>13</v>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1435,615 +1442,55 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="60.0"/>
-    <col customWidth="1" min="4" max="4" width="30.88"/>
+    <col customWidth="1" min="1" max="1" width="20.88"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="1">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="B2" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="4" t="s">
-        <v>77</v>
-      </c>
-      <c r="B3" s="1">
-        <v>2.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="B4" s="1">
-        <v>3.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B5" s="1">
-        <v>4.0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="1">
-        <v>6.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="B8" s="1">
-        <v>7.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="4" t="s">
-        <v>83</v>
-      </c>
-      <c r="B9" s="1">
-        <v>8.0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>84</v>
-      </c>
-      <c r="B10" s="1">
-        <v>9.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B11" s="1">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B12" s="1">
-        <v>11.0</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B13" s="1">
-        <v>12.0</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B14" s="1">
-        <v>13.0</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B15" s="1">
-        <v>14.0</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B16" s="1">
-        <v>15.0</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B17" s="1">
-        <v>16.0</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B18" s="1">
-        <v>17.0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="B19" s="1">
-        <v>18.0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="1">
-        <v>19.0</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="B21" s="1">
-        <v>20.0</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="B22" s="1">
-        <v>21.0</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="B23" s="1">
-        <v>22.0</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="B24" s="1">
-        <v>23.0</v>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B25" s="1">
-        <v>24.0</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="B26" s="1">
-        <v>25.0</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="B27" s="1">
-        <v>26.0</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="B28" s="1">
-        <v>27.0</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B29" s="1">
-        <v>28.0</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="B30" s="1">
-        <v>29.0</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" s="1">
-        <v>30.0</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B32" s="1">
-        <v>31.0</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B33" s="1">
-        <v>32.0</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B34" s="1">
-        <v>33.0</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B35" s="1">
-        <v>34.0</v>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="B36" s="1">
-        <v>35.0</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B37" s="1">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="B38" s="1">
-        <v>37.0</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="B39" s="1">
-        <v>38.0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="B40" s="1">
-        <v>39.0</v>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="B41" s="1">
-        <v>40.0</v>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B42" s="1">
-        <v>41.0</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B43" s="1">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B44" s="1">
-        <v>43.0</v>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B45" s="1">
-        <v>44.0</v>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B46" s="1">
-        <v>45.0</v>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B47" s="1">
-        <v>46.0</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B48" s="1">
-        <v>47.0</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="1">
-        <v>48.0</v>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B50" s="1">
-        <v>49.0</v>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B51" s="1">
-        <v>50.0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B52" s="1">
-        <v>51.0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B53" s="1">
-        <v>52.0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B54" s="1">
-        <v>53.0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B55" s="1">
-        <v>54.0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B56" s="1">
-        <v>55.0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B57" s="1">
-        <v>56.0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B58" s="1">
-        <v>57.0</v>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B59" s="1">
-        <v>58.0</v>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="B60" s="1">
-        <v>59.0</v>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="4" t="s">
-        <v>135</v>
-      </c>
-      <c r="B61" s="1">
-        <v>60.0</v>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B62" s="1">
-        <v>61.0</v>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B63" s="1">
-        <v>62.0</v>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="B64" s="1">
-        <v>63.0</v>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B65" s="1">
-        <v>64.0</v>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66" s="1">
-        <v>65.0</v>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B67" s="1">
-        <v>66.0</v>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B68" s="1">
-        <v>67.0</v>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B69" s="1">
-        <v>68.0</v>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B70" s="1">
-        <v>69.0</v>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="B71" s="1">
-        <v>70.0</v>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B72" s="1">
-        <v>71.0</v>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="B73" s="1">
-        <v>72.0</v>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="B74" s="1">
-        <v>73.0</v>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="B75" s="1">
-        <v>74.0</v>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" s="4"/>
-    </row>
-    <row r="77">
-      <c r="A77" s="4"/>
+      <c r="C2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2059,345 +1506,77 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="2" max="2" width="26.13"/>
+  </cols>
   <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>77</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>78</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="F2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>17</v>
+      <c r="A3" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>75</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -2414,46 +1593,616 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="60.0"/>
+    <col customWidth="1" min="4" max="4" width="30.88"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
+      <c r="A1" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1">
+        <v>0.0</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="A2" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="1">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B6" s="1">
+        <v>5.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="1">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1">
+        <v>8.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="1">
+        <v>9.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="1">
+        <v>10.0</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="1">
+        <v>11.0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="1">
+        <v>12.0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="1">
+        <v>13.0</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="1">
+        <v>14.0</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="1">
+        <v>15.0</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="1">
+        <v>16.0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B18" s="1">
+        <v>17.0</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B19" s="1">
+        <v>18.0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" s="1">
+        <v>19.0</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B21" s="1">
+        <v>20.0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B22" s="1">
+        <v>21.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B23" s="1">
+        <v>22.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="1">
+        <v>23.0</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B25" s="1">
+        <v>24.0</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B26" s="1">
+        <v>25.0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B27" s="1">
+        <v>26.0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B28" s="1">
+        <v>27.0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B29" s="1">
+        <v>28.0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B30" s="1">
+        <v>29.0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="1">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B32" s="1">
+        <v>31.0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B33" s="1">
+        <v>32.0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B34" s="1">
+        <v>33.0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B35" s="1">
+        <v>34.0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="1">
+        <v>35.0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B37" s="1">
+        <v>36.0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B38" s="1">
+        <v>37.0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B39" s="1">
+        <v>38.0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B40" s="1">
+        <v>39.0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B41" s="1">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B42" s="1">
+        <v>41.0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B43" s="1">
+        <v>42.0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" s="1">
+        <v>43.0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" s="1">
+        <v>44.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="1">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B47" s="1">
+        <v>46.0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="1">
+        <v>47.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B49" s="1">
+        <v>48.0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="1">
+        <v>49.0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B51" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B52" s="1">
+        <v>51.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B53" s="1">
+        <v>52.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B54" s="1">
+        <v>53.0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="B55" s="1">
+        <v>54.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B56" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B57" s="1">
+        <v>56.0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="B58" s="1">
+        <v>57.0</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B59" s="1">
+        <v>58.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="B60" s="1">
+        <v>59.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="B61" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B62" s="1">
+        <v>61.0</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B63" s="1">
+        <v>62.0</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B64" s="1">
+        <v>63.0</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="B65" s="1">
+        <v>64.0</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B66" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="B67" s="1">
+        <v>66.0</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B68" s="1">
+        <v>67.0</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="B69" s="1">
+        <v>68.0</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="B70" s="1">
+        <v>69.0</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B71" s="1">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B72" s="1">
+        <v>71.0</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="B73" s="1">
+        <v>72.0</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B74" s="1">
+        <v>73.0</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="B75" s="1">
+        <v>74.0</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" s="4"/>
+    </row>
+    <row r="77">
+      <c r="A77" s="4"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -2501,7 +2250,7 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>19</v>
@@ -2514,6 +2263,416 @@
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -2664,7 +2823,7 @@
         <v>40</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>11</v>
@@ -2681,7 +2840,7 @@
         <v>8</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>51</v>
@@ -2701,7 +2860,7 @@
         <v>8</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>55</v>
@@ -2721,7 +2880,7 @@
         <v>8</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>58</v>
@@ -2741,7 +2900,7 @@
         <v>8</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>60</v>
@@ -2761,7 +2920,7 @@
         <v>8</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>64</v>
@@ -2781,7 +2940,7 @@
         <v>8</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>67</v>
@@ -2801,7 +2960,7 @@
         <v>8</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>70</v>
@@ -2821,10 +2980,10 @@
         <v>8</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>159</v>
+        <v>163</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>160</v>
+        <v>164</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>11</v>
@@ -2841,10 +3000,10 @@
         <v>8</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>161</v>
+        <v>165</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>11</v>
@@ -2861,10 +3020,10 @@
         <v>8</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>11</v>
@@ -2881,10 +3040,10 @@
         <v>8</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>165</v>
+        <v>169</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>11</v>
@@ -2901,10 +3060,10 @@
         <v>8</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>168</v>
+        <v>172</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>11</v>
@@ -2921,10 +3080,10 @@
         <v>8</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>169</v>
+        <v>173</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>11</v>
@@ -2941,10 +3100,10 @@
         <v>8</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>171</v>
+        <v>175</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>172</v>
+        <v>176</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>11</v>
@@ -2961,10 +3120,10 @@
         <v>8</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>11</v>
@@ -2981,10 +3140,10 @@
         <v>8</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>11</v>
@@ -3001,10 +3160,10 @@
         <v>8</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="F28" s="1" t="s">
         <v>11</v>
@@ -3021,10 +3180,10 @@
         <v>8</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="F29" s="1" t="s">
         <v>11</v>
@@ -3041,10 +3200,10 @@
         <v>8</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>11</v>
@@ -3061,10 +3220,10 @@
         <v>8</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>11</v>
@@ -3081,10 +3240,10 @@
         <v>8</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="F32" s="1" t="s">
         <v>11</v>
@@ -3101,10 +3260,10 @@
         <v>8</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="F33" s="1" t="s">
         <v>11</v>
@@ -3121,10 +3280,10 @@
         <v>8</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="F34" s="1" t="s">
         <v>11</v>
@@ -3141,10 +3300,10 @@
         <v>8</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>11</v>
@@ -3161,10 +3320,10 @@
         <v>8</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>194</v>
+        <v>198</v>
       </c>
       <c r="F36" s="1" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Delete the comment lines
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -41,7 +41,7 @@
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP25617</t>
+    <t>CHAP456389</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -56,7 +56,7 @@
     <t>Avalon</t>
   </si>
   <si>
-    <t>Il75401</t>
+    <t>Il75407</t>
   </si>
   <si>
     <t>Illinois</t>
@@ -71,7 +71,7 @@
     <t>Non Prepaid</t>
   </si>
   <si>
-    <t>NC45764</t>
+    <t>NC45769</t>
   </si>
   <si>
     <t>North Carolina</t>
@@ -83,7 +83,7 @@
     <t>Echo</t>
   </si>
   <si>
-    <t>NJ75489</t>
+    <t>NJ75445</t>
   </si>
   <si>
     <t>New Jersey</t>
@@ -92,7 +92,7 @@
     <t>Walk-in</t>
   </si>
   <si>
-    <t>Il754869</t>
+    <t>Il754845</t>
   </si>
   <si>
     <t>White</t>
@@ -101,7 +101,7 @@
     <t>Camry</t>
   </si>
   <si>
-    <t>AR75488</t>
+    <t>AR75436</t>
   </si>
   <si>
     <t>Arizona</t>

</xml_diff>

<commit_message>
Cash Payment Test is successfully created
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -4,7 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="KodaWalkIn" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="ReceivePayment" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Sheet13" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="KodaWalkIn" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -12,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
   <si>
     <t>Select Source</t>
   </si>
@@ -41,7 +43,7 @@
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP456389</t>
+    <t>CHAP456304</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -60,6 +62,27 @@
   </si>
   <si>
     <t>Illinois</t>
+  </si>
+  <si>
+    <t>PaymentMode</t>
+  </si>
+  <si>
+    <t>Card Reference No</t>
+  </si>
+  <si>
+    <t>BRHM1065419</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>4242 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>BRHM1065420</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
   <si>
     <t>Reservation Prepaid</t>
@@ -111,7 +134,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -132,6 +155,10 @@
       <sz val="9.0"/>
       <color rgb="FF22191B"/>
       <name val="Monospace"/>
+    </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">
@@ -154,7 +181,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -167,6 +194,15 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -180,6 +216,14 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -459,6 +503,73 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="18.88"/>
+    <col customWidth="1" min="2" max="2" width="17.25"/>
+    <col customWidth="1" min="3" max="3" width="24.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="6">
+        <v>0.0</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="2" max="2" width="20.38"/>
   </cols>
   <sheetData>
@@ -467,7 +578,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -487,10 +598,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -502,41 +613,41 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>18</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -548,7 +659,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>
@@ -556,25 +667,25 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Card payment file test added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
   <si>
     <t>Select Source</t>
   </si>
@@ -43,7 +43,7 @@
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP456304</t>
+    <t>CHAP456312</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -70,19 +70,13 @@
     <t>Card Reference No</t>
   </si>
   <si>
-    <t>BRHM1065419</t>
+    <t>BRHM1065424</t>
   </si>
   <si>
     <t>Card</t>
   </si>
   <si>
     <t>4242 4242 4242 4242</t>
-  </si>
-  <si>
-    <t>BRHM1065420</t>
-  </si>
-  <si>
-    <t>Cash</t>
   </si>
   <si>
     <t>Reservation Prepaid</t>
@@ -201,7 +195,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,9 +497,9 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="18.88"/>
-    <col customWidth="1" min="2" max="2" width="17.25"/>
-    <col customWidth="1" min="3" max="3" width="24.63"/>
+    <col customWidth="1" min="1" max="1" width="23.0"/>
+    <col customWidth="1" min="2" max="2" width="17.63"/>
+    <col customWidth="1" min="3" max="3" width="24.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -520,7 +514,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -528,17 +522,6 @@
       </c>
       <c r="C2" s="5" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -578,7 +561,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -598,10 +581,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -613,41 +596,41 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -659,7 +642,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>
@@ -667,25 +650,25 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Demo Class file is added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -5,8 +5,9 @@
   <sheets>
     <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="ReceivePayment" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Sheet13" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="KodaWalkIn" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="UpdateReservation" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Sheet13" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="KodaWalkIn" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>Select Source</t>
   </si>
@@ -77,6 +78,15 @@
   </si>
   <si>
     <t>4242 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>Click Button</t>
+  </si>
+  <si>
+    <t>BRHM1065436</t>
+  </si>
+  <si>
+    <t>Update Reservation</t>
   </si>
   <si>
     <t>Reservation Prepaid</t>
@@ -221,6 +231,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
@@ -538,12 +552,47 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="17.25"/>
+    <col customWidth="1" min="2" max="2" width="19.63"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -561,7 +610,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
@@ -581,10 +630,10 @@
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>11</v>
@@ -596,41 +645,41 @@
         <v>13</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>11</v>
@@ -642,7 +691,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>15</v>
@@ -650,25 +699,25 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed tracked files that should be ignored
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -3,11 +3,11 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="ReceivePayment" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="UpdateReservation" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Sheet13" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="KodaWalkIn" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="KodaWalkIn" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="ThirdParty" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="ReceivePayment" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="UpdateReservation" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CheckInKeyIn" sheetId="5" r:id="rId8"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,56 +15,101 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
   <si>
     <t>Select Source</t>
   </si>
   <si>
+    <t>Reservation Prepaid</t>
+  </si>
+  <si>
+    <t>Car Color</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>License Plate</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>Koda</t>
+  </si>
+  <si>
+    <t>Non Prepaid</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Avalon</t>
+  </si>
+  <si>
+    <t>NC45769</t>
+  </si>
+  <si>
+    <t>North Carolina</t>
+  </si>
+  <si>
+    <t>Gray</t>
+  </si>
+  <si>
+    <t>Echo</t>
+  </si>
+  <si>
+    <t>NJ75445</t>
+  </si>
+  <si>
+    <t>New Jersey</t>
+  </si>
+  <si>
+    <t>Walk-in</t>
+  </si>
+  <si>
+    <t>Il754845</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Camry</t>
+  </si>
+  <si>
+    <t>AR75436</t>
+  </si>
+  <si>
+    <t>Arizona</t>
+  </si>
+  <si>
     <t>confirmation Number</t>
   </si>
   <si>
     <t>Prepaid Or Partial</t>
   </si>
   <si>
-    <t>Car Color</t>
-  </si>
-  <si>
-    <t>Make</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>License Plate</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP456312</t>
+    <t>CHAP456301</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Toyota</t>
-  </si>
-  <si>
-    <t>Avalon</t>
-  </si>
-  <si>
     <t>Il75407</t>
   </si>
   <si>
-    <t>Illinois</t>
-  </si>
-  <si>
     <t>PaymentMode</t>
   </si>
   <si>
@@ -83,55 +128,13 @@
     <t>Click Button</t>
   </si>
   <si>
-    <t>BRHM1065436</t>
+    <t>BRHM1065468</t>
   </si>
   <si>
     <t>Update Reservation</t>
   </si>
   <si>
-    <t>Reservation Prepaid</t>
-  </si>
-  <si>
-    <t>Koda</t>
-  </si>
-  <si>
-    <t>Non Prepaid</t>
-  </si>
-  <si>
-    <t>NC45769</t>
-  </si>
-  <si>
-    <t>North Carolina</t>
-  </si>
-  <si>
-    <t>Gray</t>
-  </si>
-  <si>
-    <t>Echo</t>
-  </si>
-  <si>
-    <t>NJ75445</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
-    <t>Walk-in</t>
-  </si>
-  <si>
-    <t>Il754845</t>
-  </si>
-  <si>
-    <t>White</t>
-  </si>
-  <si>
-    <t>Camry</t>
-  </si>
-  <si>
-    <t>AR75436</t>
-  </si>
-  <si>
-    <t>Arizona</t>
+    <t>Check In / Key In</t>
   </si>
 </sst>
 </file>
@@ -439,6 +442,139 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="2" max="2" width="20.38"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
     <col customWidth="1" min="1" max="1" width="33.5"/>
     <col customWidth="1" min="2" max="2" width="20.0"/>
     <col customWidth="1" min="3" max="3" width="17.25"/>
@@ -449,51 +585,51 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>8</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>13</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -501,7 +637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -518,24 +654,24 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -543,7 +679,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -553,41 +689,27 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="17.25"/>
-    <col customWidth="1" min="2" max="2" width="19.63"/>
+    <col customWidth="1" min="1" max="1" width="20.13"/>
+    <col customWidth="1" min="2" max="2" width="25.88"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>37</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -602,122 +724,23 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.38"/>
+    <col customWidth="1" min="2" max="2" width="20.63"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
+      <c r="A1" s="4" t="s">
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>7</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
+      <c r="A2" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed the ReceivePayment Data Provider
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
   <si>
     <t>Select Source</t>
   </si>
@@ -110,19 +110,56 @@
     <t>Il75407</t>
   </si>
   <si>
+    <t>Confirmation Number</t>
+  </si>
+  <si>
     <t>PaymentMode</t>
   </si>
   <si>
-    <t>Card Reference No</t>
-  </si>
-  <si>
-    <t>BRHM1065424</t>
+    <t>Card Information</t>
+  </si>
+  <si>
+    <t>Card Expiry</t>
+  </si>
+  <si>
+    <t>CVC</t>
+  </si>
+  <si>
+    <t>Billing Name</t>
+  </si>
+  <si>
+    <t>Zip</t>
+  </si>
+  <si>
+    <t>Email Id</t>
+  </si>
+  <si>
+    <t>BRHM1065534</t>
   </si>
   <si>
     <t>Card</t>
   </si>
   <si>
     <t>4242 4242 4242 4242</t>
+  </si>
+  <si>
+    <t>Meena Kumari</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <rFont val="Arial"/>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>MeenaKumari@gmail.com</t>
+    </r>
+  </si>
+  <si>
+    <t>BRHM1065535</t>
+  </si>
+  <si>
+    <t>Cash</t>
   </si>
   <si>
     <t>Click Button</t>
@@ -141,7 +178,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="d-mmm"/>
+  </numFmts>
+  <fonts count="7">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -162,6 +202,15 @@
       <sz val="9.0"/>
       <color rgb="FF22191B"/>
       <name val="Monospace"/>
+    </font>
+    <font>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
     </font>
     <font>
       <color theme="1"/>
@@ -188,7 +237,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -202,12 +251,27 @@
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -654,28 +718,69 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="4" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>33</v>
+      <c r="A2" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>35</v>
+        <v>41</v>
+      </c>
+      <c r="D2" s="6">
+        <v>45927.0</v>
+      </c>
+      <c r="E2" s="7">
+        <v>686.0</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="7">
+        <v>30048.0</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <hyperlinks>
+    <hyperlink r:id="rId1" ref="H2"/>
+  </hyperlinks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -694,19 +799,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>36</v>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>38</v>
+      <c r="A2" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -728,19 +833,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="6" t="s">
-        <v>37</v>
+      <c r="A2" s="11" t="s">
+        <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CardPayment and CashPayment Test is added
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -3,11 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="KodaWalkIn" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="ThirdParty" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
+    <sheet state="visible" name="KodaWalkIn" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="ReceivePayment" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="UpdateReservation" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CheckInKeyIn" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="Sheet20" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="CashPayment" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="UpdateReservation" sheetId="6" r:id="rId9"/>
+    <sheet state="visible" name="CheckInKeyIn" sheetId="7" r:id="rId10"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -15,71 +17,74 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
   <si>
     <t>Select Source</t>
   </si>
   <si>
+    <t>confirmation Number</t>
+  </si>
+  <si>
+    <t>Prepaid Or Partial</t>
+  </si>
+  <si>
+    <t>Car Color</t>
+  </si>
+  <si>
+    <t>Make</t>
+  </si>
+  <si>
+    <t>Model</t>
+  </si>
+  <si>
+    <t>License Plate</t>
+  </si>
+  <si>
+    <t>State</t>
+  </si>
+  <si>
+    <t>CheapAirportParking</t>
+  </si>
+  <si>
+    <t>CHAP456301</t>
+  </si>
+  <si>
+    <t>Prepaid/Partial</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>Avalon</t>
+  </si>
+  <si>
+    <t>Il75407</t>
+  </si>
+  <si>
+    <t>Illinois</t>
+  </si>
+  <si>
     <t>Reservation Prepaid</t>
   </si>
   <si>
-    <t>Car Color</t>
-  </si>
-  <si>
-    <t>Make</t>
-  </si>
-  <si>
-    <t>Model</t>
-  </si>
-  <si>
-    <t>License Plate</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>Koda</t>
   </si>
   <si>
     <t>Non Prepaid</t>
   </si>
   <si>
-    <t>Black</t>
-  </si>
-  <si>
-    <t>Toyota</t>
-  </si>
-  <si>
-    <t>Avalon</t>
-  </si>
-  <si>
     <t>NC45769</t>
   </si>
   <si>
     <t>North Carolina</t>
   </si>
   <si>
-    <t>Gray</t>
-  </si>
-  <si>
-    <t>Echo</t>
-  </si>
-  <si>
-    <t>NJ75445</t>
-  </si>
-  <si>
-    <t>New Jersey</t>
-  </si>
-  <si>
     <t>Walk-in</t>
   </si>
   <si>
-    <t>Il754845</t>
-  </si>
-  <si>
-    <t>Illinois</t>
-  </si>
-  <si>
     <t>White</t>
   </si>
   <si>
@@ -92,24 +97,6 @@
     <t>Arizona</t>
   </si>
   <si>
-    <t>confirmation Number</t>
-  </si>
-  <si>
-    <t>Prepaid Or Partial</t>
-  </si>
-  <si>
-    <t>CheapAirportParking</t>
-  </si>
-  <si>
-    <t>CHAP456301</t>
-  </si>
-  <si>
-    <t>Prepaid/Partial</t>
-  </si>
-  <si>
-    <t>Il75407</t>
-  </si>
-  <si>
     <t>Confirmation Number</t>
   </si>
   <si>
@@ -134,7 +121,7 @@
     <t>Email Id</t>
   </si>
   <si>
-    <t>BRHM1065534</t>
+    <t>BRHM1066027</t>
   </si>
   <si>
     <t>Card</t>
@@ -156,7 +143,11 @@
     </r>
   </si>
   <si>
-    <t>BRHM1065535</t>
+    <t>Confirmation Number        Payment Mode
+BRHM1066028        Cash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BRHM1066028 </t>
   </si>
   <si>
     <t>Cash</t>
@@ -181,7 +172,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="d-mmm"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -204,16 +195,12 @@
       <name val="Monospace"/>
     </font>
     <font>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <color rgb="FF0000FF"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
+      <color rgb="FF1155CC"/>
       <name val="Arial"/>
     </font>
   </fonts>
@@ -237,7 +224,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="10">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -250,29 +237,23 @@
     <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -299,6 +280,14 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -506,14 +495,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="2" max="2" width="20.38"/>
+    <col customWidth="1" min="1" max="1" width="33.5"/>
+    <col customWidth="1" min="2" max="2" width="20.0"/>
+    <col customWidth="1" min="3" max="3" width="17.25"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -531,97 +522,34 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
       <c r="D2" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -638,62 +566,74 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="33.5"/>
-    <col customWidth="1" min="2" max="2" width="20.0"/>
-    <col customWidth="1" min="3" max="3" width="17.25"/>
-  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -711,69 +651,62 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.0"/>
-    <col customWidth="1" min="2" max="2" width="17.63"/>
-    <col customWidth="1" min="3" max="3" width="24.88"/>
+    <col customWidth="1" min="1" max="1" width="17.13"/>
+    <col customWidth="1" min="2" max="2" width="18.0"/>
+    <col customWidth="1" min="3" max="3" width="17.63"/>
+    <col customWidth="1" min="4" max="4" width="19.75"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="G1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="5" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="D2" s="7">
+        <v>45927.0</v>
+      </c>
+      <c r="E2" s="8">
+        <v>686.0</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="G2" s="8">
+        <v>30048.0</v>
+      </c>
+      <c r="H2" s="9" t="s">
         <v>38</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D2" s="6">
-        <v>45927.0</v>
-      </c>
-      <c r="E2" s="7">
-        <v>686.0</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" s="7">
-        <v>30048.0</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -785,6 +718,57 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -799,19 +783,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B1" s="10" t="s">
-        <v>46</v>
+      <c r="A1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>48</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -819,7 +803,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -833,19 +817,19 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
-        <v>25</v>
+      <c r="A1" s="5" t="s">
+        <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="11" t="s">
-        <v>47</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Validate the due Amount in Create Reservation
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/ExcelTestData.xlsx
+++ b/src/test/resources/TestData/ExcelTestData.xlsx
@@ -6,10 +6,9 @@
     <sheet state="visible" name="ThirdParty" sheetId="1" r:id="rId4"/>
     <sheet state="visible" name="KodaWalkIn" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="ReceivePayment" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Sheet20" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="CashPayment" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="UpdateReservation" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="CheckInKeyIn" sheetId="7" r:id="rId10"/>
+    <sheet state="visible" name="CashPayment" sheetId="4" r:id="rId7"/>
+    <sheet state="visible" name="UpdateReservation" sheetId="5" r:id="rId8"/>
+    <sheet state="visible" name="CheckInKeyIn" sheetId="6" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -17,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="45">
   <si>
     <t>Select Source</t>
   </si>
@@ -46,7 +45,7 @@
     <t>CheapAirportParking</t>
   </si>
   <si>
-    <t>CHAP456301</t>
+    <t>CHAP456347</t>
   </si>
   <si>
     <t>Prepaid/Partial</t>
@@ -121,7 +120,7 @@
     <t>Email Id</t>
   </si>
   <si>
-    <t>BRHM1066027</t>
+    <t>BRHM1166048</t>
   </si>
   <si>
     <t>Card</t>
@@ -143,11 +142,7 @@
     </r>
   </si>
   <si>
-    <t>Confirmation Number        Payment Mode
-BRHM1066028        Cash</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BRHM1066028 </t>
+    <t>BRHM1166047</t>
   </si>
   <si>
     <t>Cash</t>
@@ -156,10 +151,10 @@
     <t>Click Button</t>
   </si>
   <si>
-    <t>BRHM1065468</t>
-  </si>
-  <si>
     <t>Update Reservation</t>
+  </si>
+  <si>
+    <t>BRHM1166045</t>
   </si>
   <si>
     <t>Check In / Key In</t>
@@ -284,10 +279,6 @@
 </file>
 
 <file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -728,8 +719,19 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="s">
         <v>39</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -738,37 +740,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -787,15 +758,15 @@
         <v>1</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -803,7 +774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -821,7 +792,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2">
@@ -829,7 +800,7 @@
         <v>43</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>